<commit_message>
Modify to extract initial main texts and borderless table more accurately
</commit_message>
<xml_diff>
--- a/output/page_1.xlsx
+++ b/output/page_1.xlsx
@@ -11,6 +11,122 @@
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+  <si>
+    <t>MASTER PACKAGE</t>
+  </si>
+  <si>
+    <t>WesternGlove Centric8 PROD</t>
+  </si>
+  <si>
+    <t>M12225BVS563:KONRAD</t>
+  </si>
+  <si>
+    <t>FRONT AND BACK SKETCH</t>
+  </si>
+  <si>
+    <t>MASTER</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>ASM-VN</t>
+  </si>
+  <si>
+    <t>Collection</t>
+  </si>
+  <si>
+    <t>LONG BOTTOMS (20)</t>
+  </si>
+  <si>
+    <t>Season</t>
+  </si>
+  <si>
+    <t>2025 - Q3 - FALL</t>
+  </si>
+  <si>
+    <t>Division</t>
+  </si>
+  <si>
+    <t>SILVER JEANS CO.</t>
+  </si>
+  <si>
+    <t>Sub Division</t>
+  </si>
+  <si>
+    <t>Cut #</t>
+  </si>
+  <si>
+    <t>Pattern #</t>
+  </si>
+  <si>
+    <t>M12225BVSCONTJANO325WG</t>
+  </si>
+  <si>
+    <t>Default Color</t>
+  </si>
+  <si>
+    <t>DUNE WASH</t>
+  </si>
+  <si>
+    <t>SJC Program</t>
+  </si>
+  <si>
+    <t>DESK TO DINNER</t>
+  </si>
+  <si>
+    <t>ECO Wash</t>
+  </si>
+  <si>
+    <t>No ECO Wash</t>
+  </si>
+  <si>
+    <t>Rise</t>
+  </si>
+  <si>
+    <t>SITS BELOW WAIST</t>
+  </si>
+  <si>
+    <t>Fit Description (new)</t>
+  </si>
+  <si>
+    <t>SLIM FIT</t>
+  </si>
+  <si>
+    <t>Leg Description</t>
+  </si>
+  <si>
+    <t>SLIM LEG</t>
+  </si>
+  <si>
+    <t>Created</t>
+  </si>
+  <si>
+    <t>5/21/24, 4:00 PM</t>
+  </si>
+  <si>
+    <t>Created By</t>
+  </si>
+  <si>
+    <t>Brodie Silver</t>
+  </si>
+  <si>
+    <t>Modified</t>
+  </si>
+  <si>
+    <t>1/14/25, 4:05 PM</t>
+  </si>
+  <si>
+    <t>Modified By</t>
+  </si>
+  <si>
+    <t>Sincere Santos</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -32,7 +148,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -40,12 +156,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -340,12 +474,237 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modify to extract 2 initial lines of main texts the other way, to extract table more accurately and add lines formats like in images
</commit_message>
<xml_diff>
--- a/output/page_1.xlsx
+++ b/output/page_1.xlsx
@@ -7,28 +7,19 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="page_1 - Table 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
-  <si>
-    <t>MASTER PACKAGE</t>
-  </si>
-  <si>
-    <t>WesternGlove Centric8 PROD</t>
-  </si>
-  <si>
-    <t>M12225BVS563:KONRAD</t>
-  </si>
-  <si>
-    <t>FRONT AND BACK SKETCH</t>
-  </si>
-  <si>
-    <t>MASTER</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+  <si>
+    <t xml:space="preserve"> MASTER PACKAGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> WesternGlove Centric8 PROD                                     M12225BVS563:KONRAD                                 FRONT AND BACK SKETCH                                 MASTER</t>
   </si>
   <si>
     <t>Code</t>
@@ -131,9 +122,24 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -175,8 +181,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -474,233 +486,273 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:Z21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1"/>
+    <col min="4" max="4" width="38" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+    </row>
+    <row r="2" spans="1:26">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+    </row>
+    <row r="4" spans="1:26">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+    </row>
+    <row r="5" spans="1:26">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
+      <c r="E5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="1" t="s">
+    </row>
+    <row r="6" spans="1:26">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
+      <c r="E6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="1" t="s">
+    </row>
+    <row r="7" spans="1:26">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
+      <c r="E7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="1" t="s">
+    </row>
+    <row r="8" spans="1:26">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1" t="s">
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:26">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:26">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
+      <c r="E10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1" t="s">
+    </row>
+    <row r="11" spans="1:26">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1" t="s">
+      <c r="E11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="1" t="s">
+    </row>
+    <row r="12" spans="1:26">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1" t="s">
+      <c r="E12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="1" t="s">
+    </row>
+    <row r="13" spans="1:26">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1" t="s">
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:26">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:26">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1" t="s">
+      <c r="E15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1" t="s">
+    </row>
+    <row r="16" spans="1:26">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1" t="s">
+      <c r="E16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="1" t="s">
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1" t="s">
+      <c r="E17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="1" t="s">
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1" t="s">
+      <c r="E18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="1" t="s">
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1" t="s">
+      <c r="E19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="1" t="s">
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1" t="s">
+      <c r="E20" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="1" t="s">
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1" t="s">
+      <c r="E21" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>36</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
+    <mergeCell ref="A1:Z1"/>
+    <mergeCell ref="A2:Z2"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>

</xml_diff>